<commit_message>
updated full analysis; tbc
</commit_message>
<xml_diff>
--- a/outputs/excel/x_comparison_four_models.xlsx
+++ b/outputs/excel/x_comparison_four_models.xlsx
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="C7" t="n">
         <v>0.38</v>
@@ -1444,7 +1444,6 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
           <t>nan</t>
@@ -1521,7 +1520,6 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
           <t>nan</t>

</xml_diff>

<commit_message>
Comparing all four models
</commit_message>
<xml_diff>
--- a/outputs/excel/x_comparison_four_models.xlsx
+++ b/outputs/excel/x_comparison_four_models.xlsx
@@ -13,6 +13,10 @@
     <sheet name="PostSummary_TRI_M1" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="PostSummary_TRI_M2" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="ModelFit_Table" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Bi_Convergence_M1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Bi_Convergence_M2" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Tri_Convergence_M1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Tri_Convergence_M2" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -541,6 +545,378 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>sd</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>hdi_3%</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>hdi_97%</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>mcse_mean</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>mcse_sd</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ess_bulk</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ess_tail</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>r_hat</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>level_2[log_lambda (intercept)]</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-3.6485</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1213</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-3.8855</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-3.4181</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0128</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0083</v>
+      </c>
+      <c r="H2" t="n">
+        <v>92.5595</v>
+      </c>
+      <c r="I2" t="n">
+        <v>71.0873</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.0542</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>level_2[log_mu (intercept)]</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.07149999999999999</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.2403</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0297</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0028</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0022</v>
+      </c>
+      <c r="H3" t="n">
+        <v>685.2626</v>
+      </c>
+      <c r="I3" t="n">
+        <v>855.3287</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.0067</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>level_2[log_eta (intercept)]</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.0898</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.08160000000000001</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.0643</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.2443</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H4" t="n">
+        <v>329.423</v>
+      </c>
+      <c r="I4" t="n">
+        <v>611.2028</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.0045</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>level_2[var_log_lambda]</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1.4108</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1682</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.1147</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.7525</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0164</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0104</v>
+      </c>
+      <c r="H5" t="n">
+        <v>105.5862</v>
+      </c>
+      <c r="I5" t="n">
+        <v>155.579</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.0353</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>level_2[cov_log_lambda_mu]</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1998</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.2445</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.2363</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.6497000000000001</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0261</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="H6" t="n">
+        <v>95.3501</v>
+      </c>
+      <c r="I6" t="n">
+        <v>97.31440000000001</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.0352</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>level_2[cov_log_lambda_eta]</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0152</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0105</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.0047</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0347</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="H7" t="n">
+        <v>9819.058300000001</v>
+      </c>
+      <c r="I7" t="n">
+        <v>9666.892900000001</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.001</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>level_2[var_log_mu]</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2.0188</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.8012</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.8609</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.5449</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.172</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.07389999999999999</v>
+      </c>
+      <c r="H8" t="n">
+        <v>21.7429</v>
+      </c>
+      <c r="I8" t="n">
+        <v>93.524</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.1361</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>level_2[cov_log_mu_eta]</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.0062</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0131</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0.0306</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.0188</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1141.9562</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1309.9337</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.0071</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>level_2[var_log_eta]</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0752</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.1124</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="H10" t="n">
+        <v>478.6025</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1363.5061</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.0101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -907,13 +1283,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-3.76</v>
+        <v>-3.75</v>
       </c>
       <c r="C2" t="n">
-        <v>-3.59</v>
+        <v>-3.5</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.41</v>
+        <v>-3.24</v>
       </c>
     </row>
     <row r="3">
@@ -923,13 +1299,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-4.03</v>
+        <v>-4.18</v>
       </c>
       <c r="C3" t="n">
-        <v>-3.68</v>
+        <v>-3.64</v>
       </c>
       <c r="D3" t="n">
-        <v>-3.34</v>
+        <v>-3.18</v>
       </c>
     </row>
     <row r="4">
@@ -955,13 +1331,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.15</v>
+        <v>1.01</v>
       </c>
       <c r="C5" t="n">
-        <v>1.42</v>
+        <v>1.36</v>
       </c>
       <c r="D5" t="n">
-        <v>1.72</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="6">
@@ -971,13 +1347,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.14</v>
+        <v>-0.2</v>
       </c>
       <c r="C6" t="n">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="D6" t="n">
-        <v>0.65</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="7">
@@ -1003,13 +1379,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.89</v>
+        <v>1.02</v>
       </c>
       <c r="C8" t="n">
-        <v>2.26</v>
+        <v>3.07</v>
       </c>
       <c r="D8" t="n">
-        <v>4.08</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="9">
@@ -1019,7 +1395,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="C9" t="n">
         <v>-0.01</v>
@@ -1041,7 +1417,7 @@
         <v>0.08</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
   </sheetData>
@@ -1087,13 +1463,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-3.83</v>
+        <v>-3.82</v>
       </c>
       <c r="C2" t="n">
-        <v>-3.61</v>
+        <v>-3.64</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.41</v>
+        <v>-3.46</v>
       </c>
     </row>
     <row r="3">
@@ -1103,13 +1479,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.24</v>
+        <v>-0.23</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.09</v>
+        <v>-0.1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="4">
@@ -1119,13 +1495,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.08</v>
+        <v>-0.06</v>
       </c>
       <c r="C4" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="D4" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="5">
@@ -1135,13 +1511,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-4.35</v>
+        <v>-4.29</v>
       </c>
       <c r="C5" t="n">
-        <v>-3.84</v>
+        <v>-3.91</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.5</v>
+        <v>-3.58</v>
       </c>
     </row>
     <row r="6">
@@ -1151,13 +1527,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="C6" t="n">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="D6" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="7">
@@ -1167,13 +1543,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0</v>
+        <v>0.03</v>
       </c>
       <c r="C7" t="n">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="D7" t="n">
-        <v>0.79</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="8">
@@ -1189,7 +1565,7 @@
         <v>3.21</v>
       </c>
       <c r="D8" t="n">
-        <v>3.38</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="9">
@@ -1199,13 +1575,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.23</v>
+        <v>-0.22</v>
       </c>
       <c r="C9" t="n">
         <v>0.01</v>
       </c>
       <c r="D9" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="10">
@@ -1231,13 +1607,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.11</v>
+        <v>1.17</v>
       </c>
       <c r="C11" t="n">
-        <v>1.36</v>
+        <v>1.4</v>
       </c>
       <c r="D11" t="n">
-        <v>1.72</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="12">
@@ -1247,13 +1623,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.19</v>
+        <v>-0.13</v>
       </c>
       <c r="C12" t="n">
         <v>0.18</v>
       </c>
       <c r="D12" t="n">
-        <v>0.65</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="13">
@@ -1279,13 +1655,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.18</v>
+        <v>1.01</v>
       </c>
       <c r="C14" t="n">
-        <v>2.39</v>
+        <v>1.94</v>
       </c>
       <c r="D14" t="n">
-        <v>4.29</v>
+        <v>3.89</v>
       </c>
     </row>
     <row r="15">
@@ -1295,7 +1671,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.04</v>
+        <v>-0.03</v>
       </c>
       <c r="C15" t="n">
         <v>-0.01</v>
@@ -1317,7 +1693,7 @@
         <v>0.09</v>
       </c>
       <c r="D16" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
     </row>
   </sheetData>
@@ -1434,12 +1810,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.98</t>
+          <t>0.99</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.98</t>
+          <t>0.97</t>
         </is>
       </c>
     </row>
@@ -1488,7 +1864,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2.66</t>
+          <t>2.65</t>
         </is>
       </c>
     </row>
@@ -1510,12 +1886,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.74</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.77</t>
+          <t>0.80</t>
         </is>
       </c>
     </row>
@@ -1613,12 +1989,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>11.21</t>
+          <t>10.75</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>11.64</t>
+          <t>11.90</t>
         </is>
       </c>
     </row>
@@ -1640,12 +2016,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6.95</t>
+          <t>6.96</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6.91</t>
+          <t>6.86</t>
         </is>
       </c>
     </row>
@@ -1667,13 +2043,1061 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>6.68</t>
+          <t>6.57</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>6.75</t>
-        </is>
+          <t>6.77</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>sd</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>hdi_3%</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>hdi_97%</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>mcse_mean</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>mcse_sd</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ess_bulk</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ess_tail</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>r_hat</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>level_2[log_lambda (intercept)]</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-3.5444</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1033</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-3.7341</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-3.3423</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0055</v>
+      </c>
+      <c r="H2" t="n">
+        <v>55.0324</v>
+      </c>
+      <c r="I2" t="n">
+        <v>169.1281</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.0379</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>level_2[log_mu (intercept)]</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-3.6375</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1906</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-4.0056</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-3.2987</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0209</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0124</v>
+      </c>
+      <c r="H3" t="n">
+        <v>82.32940000000001</v>
+      </c>
+      <c r="I3" t="n">
+        <v>92.0359</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.0553</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>level_2[var_log_lambda]</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1.3788</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.151</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.1081</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.6683</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0151</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="H4" t="n">
+        <v>101.3883</v>
+      </c>
+      <c r="I4" t="n">
+        <v>266.408</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.024</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>level_2[cov_log_lambda_mu]</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.217</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.2602</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.2543</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6837</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0399</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="H5" t="n">
+        <v>49.3175</v>
+      </c>
+      <c r="I5" t="n">
+        <v>92.5549</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.0754</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>level_2[var_log_mu]</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2.9116</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.1705</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5.0425</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.2164</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.191</v>
+      </c>
+      <c r="H6" t="n">
+        <v>28.2635</v>
+      </c>
+      <c r="I6" t="n">
+        <v>28.4597</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.1032</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>sd</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>hdi_3%</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>hdi_97%</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>mcse_mean</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>mcse_sd</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ess_bulk</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ess_tail</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>r_hat</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>level_2[log_lambda (intercept)]</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-3.64</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1254</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-3.8672</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-3.3988</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0226</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0044</v>
+      </c>
+      <c r="H2" t="n">
+        <v>30.9104</v>
+      </c>
+      <c r="I2" t="n">
+        <v>244.0368</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.0877</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>level_2[log_mu (intercept)]</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.2056</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.3069</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0031</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0013</v>
+      </c>
+      <c r="H3" t="n">
+        <v>348.7436</v>
+      </c>
+      <c r="I3" t="n">
+        <v>710.9018</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.0133</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>level_2[beta_lambda[0]]</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-0.1051</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0743</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.2497</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0303</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0023</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1063.5685</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1859.6704</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.0074</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>level_2[beta_mu[0]]</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.08400000000000001</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0927</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.0887</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.2634</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0043</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0021</v>
+      </c>
+      <c r="H5" t="n">
+        <v>461.2482</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1018.5832</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.0052</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>level_2[beta_lambda[1]]</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-3.9504</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.2648</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-4.4472</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-3.4679</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0381</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="H6" t="n">
+        <v>48.8896</v>
+      </c>
+      <c r="I6" t="n">
+        <v>186.3261</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.0679</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>level_2[beta_mu[1]]</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0486</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1299</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.2886</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.007900000000000001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0052</v>
+      </c>
+      <c r="H7" t="n">
+        <v>268.9322</v>
+      </c>
+      <c r="I7" t="n">
+        <v>402.8904</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.0221</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>level_2[beta_lambda[2]]</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.09669999999999999</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1068</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-0.1011</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.2961</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0059</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="H8" t="n">
+        <v>322.6393</v>
+      </c>
+      <c r="I8" t="n">
+        <v>629.7186</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.0217</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>level_2[beta_mu[2]]</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.4295</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.2289</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0081</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.8832</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0141</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="H9" t="n">
+        <v>265.7637</v>
+      </c>
+      <c r="I9" t="n">
+        <v>546.0699</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.0103</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>level_2[var_log_lambda]</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1.3803</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.1672</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.0688</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.6917</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0068</v>
+      </c>
+      <c r="H10" t="n">
+        <v>32.6989</v>
+      </c>
+      <c r="I10" t="n">
+        <v>205.9711</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.0876</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>level_2[cov_log_lambda_mu]</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.2055</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.2367</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.2348</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.6422</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0303</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0149</v>
+      </c>
+      <c r="H11" t="n">
+        <v>57.7232</v>
+      </c>
+      <c r="I11" t="n">
+        <v>136.898</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.0641</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>level_2[var_log_mu]</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2.3503</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.0039</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.668</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4.3239</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.1511</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0717</v>
+      </c>
+      <c r="H12" t="n">
+        <v>40.4364</v>
+      </c>
+      <c r="I12" t="n">
+        <v>97.0141</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1.0794</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>sd</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>hdi_3%</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>hdi_97%</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>mcse_mean</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>mcse_sd</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ess_bulk</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ess_tail</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>r_hat</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>level_2[log_lambda (intercept)]</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-3.5331</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1106</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-3.7339</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-3.3262</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0209</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0067</v>
+      </c>
+      <c r="H2" t="n">
+        <v>28.4573</v>
+      </c>
+      <c r="I2" t="n">
+        <v>115.1459</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>level_2[log_mu (intercept)]</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-3.6239</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1963</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-3.9877</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-3.2549</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0219</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0143</v>
+      </c>
+      <c r="H3" t="n">
+        <v>81.2829</v>
+      </c>
+      <c r="I3" t="n">
+        <v>140.7322</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.0492</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>level_2[log_eta (intercept)]</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3.2314</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0149</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3.2022</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3.2582</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1499.9869</v>
+      </c>
+      <c r="I4" t="n">
+        <v>3149.9149</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.0011</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>level_2[var_log_lambda]</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1.3561</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1565</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0612</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.6539</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0152</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0074</v>
+      </c>
+      <c r="H5" t="n">
+        <v>104.6756</v>
+      </c>
+      <c r="I5" t="n">
+        <v>192.2475</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.0205</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>level_2[cov_log_lambda_mu]</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.2242</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.2678</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.2462</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.7141</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0506</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H6" t="n">
+        <v>38.5095</v>
+      </c>
+      <c r="I6" t="n">
+        <v>34.83</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.0935</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>level_2[cov_log_lambda_eta]</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0131</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.009900000000000001</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.0054</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0318</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="H7" t="n">
+        <v>6127.531</v>
+      </c>
+      <c r="I7" t="n">
+        <v>12502.7976</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.0014</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>level_2[var_log_mu]</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2.8646</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.2543</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.0011</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5.367</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.3966</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1627</v>
+      </c>
+      <c r="H8" t="n">
+        <v>11.0432</v>
+      </c>
+      <c r="I8" t="n">
+        <v>66.8747</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.2849</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>level_2[cov_log_mu_eta]</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.008200000000000001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0147</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0.0368</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.0188</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1379.3299</v>
+      </c>
+      <c r="I9" t="n">
+        <v>636.0331</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.0141</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>level_2[var_log_eta]</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.08450000000000001</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0098</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0667</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.1033</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="H10" t="n">
+        <v>510.1431</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1001.5409</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.0083</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increased burnin, draws mh steps
</commit_message>
<xml_diff>
--- a/outputs/excel/x_comparison_four_models.xlsx
+++ b/outputs/excel/x_comparison_four_models.xlsx
@@ -613,31 +613,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-3.6485</v>
+        <v>-3.6304</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1213</v>
+        <v>0.1217</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.8855</v>
+        <v>-3.8555</v>
       </c>
       <c r="E2" t="n">
-        <v>-3.4181</v>
+        <v>-3.3976</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0128</v>
+        <v>0.0134</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0083</v>
+        <v>0.0043</v>
       </c>
       <c r="H2" t="n">
-        <v>92.5595</v>
+        <v>83.1588</v>
       </c>
       <c r="I2" t="n">
-        <v>71.0873</v>
+        <v>262.4961</v>
       </c>
       <c r="J2" t="n">
-        <v>1.0542</v>
+        <v>1.0496</v>
       </c>
     </row>
     <row r="3">
@@ -647,31 +647,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.1</v>
+        <v>-0.0993</v>
       </c>
       <c r="C3" t="n">
-        <v>0.07149999999999999</v>
+        <v>0.0709</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.2403</v>
+        <v>-0.2312</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0297</v>
+        <v>0.0357</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0028</v>
+        <v>0.0017</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0022</v>
+        <v>0.0011</v>
       </c>
       <c r="H3" t="n">
-        <v>685.2626</v>
+        <v>1663.7939</v>
       </c>
       <c r="I3" t="n">
-        <v>855.3287</v>
+        <v>3836.1885</v>
       </c>
       <c r="J3" t="n">
-        <v>1.0067</v>
+        <v>1.0022</v>
       </c>
     </row>
     <row r="4">
@@ -681,31 +681,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0898</v>
+        <v>0.08359999999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>0.08160000000000001</v>
+        <v>0.0795</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.0643</v>
+        <v>-0.0635</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2443</v>
+        <v>0.2343</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0045</v>
+        <v>0.0029</v>
       </c>
       <c r="G4" t="n">
-        <v>0.002</v>
+        <v>0.0014</v>
       </c>
       <c r="H4" t="n">
-        <v>329.423</v>
+        <v>742.2295</v>
       </c>
       <c r="I4" t="n">
-        <v>611.2028</v>
+        <v>1727.2252</v>
       </c>
       <c r="J4" t="n">
-        <v>1.0045</v>
+        <v>1.0031</v>
       </c>
     </row>
     <row r="5">
@@ -715,31 +715,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.4108</v>
+        <v>1.3893</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1682</v>
+        <v>0.162</v>
       </c>
       <c r="D5" t="n">
-        <v>1.1147</v>
+        <v>1.0976</v>
       </c>
       <c r="E5" t="n">
-        <v>1.7525</v>
+        <v>1.7093</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0164</v>
+        <v>0.0145</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0104</v>
+        <v>0.0049</v>
       </c>
       <c r="H5" t="n">
-        <v>105.5862</v>
+        <v>124.3793</v>
       </c>
       <c r="I5" t="n">
-        <v>155.579</v>
+        <v>408.853</v>
       </c>
       <c r="J5" t="n">
-        <v>1.0353</v>
+        <v>1.042</v>
       </c>
     </row>
     <row r="6">
@@ -749,31 +749,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1998</v>
+        <v>0.1718</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2445</v>
+        <v>0.2085</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.2363</v>
+        <v>-0.2143</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6497000000000001</v>
+        <v>0.5675</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0261</v>
+        <v>0.0153</v>
       </c>
       <c r="G6" t="n">
-        <v>0.029</v>
+        <v>0.0078</v>
       </c>
       <c r="H6" t="n">
-        <v>95.3501</v>
+        <v>182.3889</v>
       </c>
       <c r="I6" t="n">
-        <v>97.31440000000001</v>
+        <v>428.4539</v>
       </c>
       <c r="J6" t="n">
-        <v>1.0352</v>
+        <v>1.0241</v>
       </c>
     </row>
     <row r="7">
@@ -783,31 +783,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0152</v>
+        <v>0.0151</v>
       </c>
       <c r="C7" t="n">
         <v>0.0105</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0047</v>
+        <v>-0.0044</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0347</v>
+        <v>0.0352</v>
       </c>
       <c r="F7" t="n">
         <v>0.0001</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>9819.058300000001</v>
+        <v>10735.968</v>
       </c>
       <c r="I7" t="n">
-        <v>9666.892900000001</v>
+        <v>21456.001</v>
       </c>
       <c r="J7" t="n">
-        <v>1.001</v>
+        <v>1.0019</v>
       </c>
     </row>
     <row r="8">
@@ -817,31 +817,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.0188</v>
+        <v>2.1195</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8012</v>
+        <v>0.9838</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8609</v>
+        <v>0.4981</v>
       </c>
       <c r="E8" t="n">
-        <v>3.5449</v>
+        <v>3.9412</v>
       </c>
       <c r="F8" t="n">
-        <v>0.172</v>
+        <v>0.1608</v>
       </c>
       <c r="G8" t="n">
-        <v>0.07389999999999999</v>
+        <v>0.0732</v>
       </c>
       <c r="H8" t="n">
-        <v>21.7429</v>
+        <v>36.4652</v>
       </c>
       <c r="I8" t="n">
-        <v>93.524</v>
+        <v>112.901</v>
       </c>
       <c r="J8" t="n">
-        <v>1.1361</v>
+        <v>1.0934</v>
       </c>
     </row>
     <row r="9">
@@ -851,16 +851,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.0062</v>
+        <v>-0.0072</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0131</v>
+        <v>0.0135</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.0306</v>
+        <v>-0.0335</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0188</v>
+        <v>0.0175</v>
       </c>
       <c r="F9" t="n">
         <v>0.0004</v>
@@ -869,13 +869,13 @@
         <v>0.0004</v>
       </c>
       <c r="H9" t="n">
-        <v>1141.9562</v>
+        <v>1020.2956</v>
       </c>
       <c r="I9" t="n">
-        <v>1309.9337</v>
+        <v>1310.9524</v>
       </c>
       <c r="J9" t="n">
-        <v>1.0071</v>
+        <v>1.0063</v>
       </c>
     </row>
     <row r="10">
@@ -885,31 +885,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.094</v>
+        <v>0.09470000000000001</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01</v>
+        <v>0.009900000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0752</v>
+        <v>0.0766</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1124</v>
+        <v>0.1135</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0005</v>
+        <v>0.0003</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0002</v>
+        <v>0.0001</v>
       </c>
       <c r="H10" t="n">
-        <v>478.6025</v>
+        <v>1292.2827</v>
       </c>
       <c r="I10" t="n">
-        <v>1363.5061</v>
+        <v>2693.9331</v>
       </c>
       <c r="J10" t="n">
-        <v>1.0101</v>
+        <v>1.0013</v>
       </c>
     </row>
   </sheetData>
@@ -955,13 +955,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-3.71</v>
+        <v>-3.78</v>
       </c>
       <c r="C2" t="n">
-        <v>-3.53</v>
+        <v>-3.56</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.35</v>
+        <v>-3.37</v>
       </c>
     </row>
     <row r="3">
@@ -971,10 +971,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-4.05</v>
+        <v>-4.07</v>
       </c>
       <c r="C3" t="n">
-        <v>-3.66</v>
+        <v>-3.65</v>
       </c>
       <c r="D3" t="n">
         <v>-3.33</v>
@@ -987,13 +987,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.13</v>
+        <v>1.14</v>
       </c>
       <c r="C4" t="n">
-        <v>1.37</v>
+        <v>1.39</v>
       </c>
       <c r="D4" t="n">
-        <v>1.68</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="5">
@@ -1003,13 +1003,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.15</v>
+        <v>-0.17</v>
       </c>
       <c r="C5" t="n">
-        <v>0.28</v>
+        <v>0.21</v>
       </c>
       <c r="D5" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6">
@@ -1019,13 +1019,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.01</v>
+        <v>0.84</v>
       </c>
       <c r="C6" t="n">
-        <v>2.94</v>
+        <v>2.6</v>
       </c>
       <c r="D6" t="n">
-        <v>5.45</v>
+        <v>5.63</v>
       </c>
     </row>
   </sheetData>
@@ -1071,13 +1071,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-3.88</v>
+        <v>-3.87</v>
       </c>
       <c r="C2" t="n">
         <v>-3.65</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.35</v>
+        <v>-3.41</v>
       </c>
     </row>
     <row r="3">
@@ -1093,7 +1093,7 @@
         <v>0.2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="4">
@@ -1109,7 +1109,7 @@
         <v>-0.1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="5">
@@ -1122,10 +1122,10 @@
         <v>-0.1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>0.29</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="6">
@@ -1135,13 +1135,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-4.54</v>
+        <v>-4.46</v>
       </c>
       <c r="C6" t="n">
-        <v>-3.95</v>
+        <v>-3.91</v>
       </c>
       <c r="D6" t="n">
-        <v>-3.46</v>
+        <v>-3.53</v>
       </c>
     </row>
     <row r="7">
@@ -1151,7 +1151,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.24</v>
+        <v>-0.26</v>
       </c>
       <c r="C7" t="n">
         <v>0.04</v>
@@ -1167,13 +1167,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.1</v>
+        <v>-0.12</v>
       </c>
       <c r="C8" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="D8" t="n">
-        <v>0.31</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="9">
@@ -1186,10 +1186,10 @@
         <v>-0.03</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4</v>
+        <v>0.37</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="10">
@@ -1199,13 +1199,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.04</v>
+        <v>1.1</v>
       </c>
       <c r="C10" t="n">
         <v>1.38</v>
       </c>
       <c r="D10" t="n">
-        <v>1.76</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="11">
@@ -1215,13 +1215,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.18</v>
+        <v>-0.23</v>
       </c>
       <c r="C11" t="n">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
       <c r="D11" t="n">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="12">
@@ -1231,13 +1231,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.96</v>
+        <v>0.71</v>
       </c>
       <c r="C12" t="n">
-        <v>2.24</v>
+        <v>2.06</v>
       </c>
       <c r="D12" t="n">
-        <v>4.81</v>
+        <v>4.82</v>
       </c>
     </row>
   </sheetData>
@@ -1283,13 +1283,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-3.75</v>
+        <v>-3.8</v>
       </c>
       <c r="C2" t="n">
-        <v>-3.5</v>
+        <v>-3.57</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.24</v>
+        <v>-3.37</v>
       </c>
     </row>
     <row r="3">
@@ -1299,13 +1299,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-4.18</v>
+        <v>-4.23</v>
       </c>
       <c r="C3" t="n">
-        <v>-3.64</v>
+        <v>-3.68</v>
       </c>
       <c r="D3" t="n">
-        <v>-3.18</v>
+        <v>-3.26</v>
       </c>
     </row>
     <row r="4">
@@ -1331,13 +1331,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.01</v>
+        <v>1.09</v>
       </c>
       <c r="C5" t="n">
-        <v>1.36</v>
+        <v>1.39</v>
       </c>
       <c r="D5" t="n">
-        <v>1.74</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="6">
@@ -1347,13 +1347,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.2</v>
+        <v>-0.23</v>
       </c>
       <c r="C6" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="D6" t="n">
-        <v>1.16</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="7">
@@ -1379,13 +1379,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.02</v>
+        <v>1.16</v>
       </c>
       <c r="C8" t="n">
-        <v>3.07</v>
+        <v>2.5</v>
       </c>
       <c r="D8" t="n">
-        <v>6.4</v>
+        <v>4.57</v>
       </c>
     </row>
     <row r="9">
@@ -1417,7 +1417,7 @@
         <v>0.08</v>
       </c>
       <c r="D10" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -1463,13 +1463,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-3.82</v>
+        <v>-3.83</v>
       </c>
       <c r="C2" t="n">
-        <v>-3.64</v>
+        <v>-3.59</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.46</v>
+        <v>-3.35</v>
       </c>
     </row>
     <row r="3">
@@ -1479,13 +1479,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.23</v>
+        <v>-0.25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
       <c r="D3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4">
@@ -1495,13 +1495,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.06</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="C4" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="D4" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="5">
@@ -1511,13 +1511,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-4.29</v>
+        <v>-4.28</v>
       </c>
       <c r="C5" t="n">
-        <v>-3.91</v>
+        <v>-3.82</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.58</v>
+        <v>-3.47</v>
       </c>
     </row>
     <row r="6">
@@ -1527,13 +1527,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-0.09</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="7">
@@ -1543,13 +1543,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="D7" t="n">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="8">
@@ -1559,7 +1559,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3.03</v>
+        <v>3.04</v>
       </c>
       <c r="C8" t="n">
         <v>3.21</v>
@@ -1578,10 +1578,10 @@
         <v>-0.22</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D9" t="n">
-        <v>0.24</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="10">
@@ -1591,7 +1591,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="C10" t="n">
         <v>0.04</v>
@@ -1607,13 +1607,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.17</v>
+        <v>1.06</v>
       </c>
       <c r="C11" t="n">
-        <v>1.4</v>
+        <v>1.34</v>
       </c>
       <c r="D11" t="n">
-        <v>1.69</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="12">
@@ -1623,13 +1623,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.13</v>
+        <v>-0.17</v>
       </c>
       <c r="C12" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="D12" t="n">
-        <v>0.72</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="13">
@@ -1645,7 +1645,7 @@
         <v>0.01</v>
       </c>
       <c r="D13" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="14">
@@ -1655,13 +1655,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.01</v>
+        <v>0.8</v>
       </c>
       <c r="C14" t="n">
-        <v>1.94</v>
+        <v>2.4</v>
       </c>
       <c r="D14" t="n">
-        <v>3.89</v>
+        <v>4.84</v>
       </c>
     </row>
     <row r="15">
@@ -1671,7 +1671,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="C15" t="n">
         <v>-0.01</v>
@@ -1693,7 +1693,7 @@
         <v>0.09</v>
       </c>
       <c r="D16" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.97</t>
+          <t>0.98</t>
         </is>
       </c>
     </row>
@@ -1864,7 +1864,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2.65</t>
+          <t>2.66</t>
         </is>
       </c>
     </row>
@@ -1881,17 +1881,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.74</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.74</t>
+          <t>0.75</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.80</t>
+          <t>0.79</t>
         </is>
       </c>
     </row>
@@ -1979,22 +1979,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10.44</t>
+          <t>10.49</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>11.05</t>
+          <t>10.73</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>10.75</t>
+          <t>10.94</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>11.90</t>
+          <t>11.94</t>
         </is>
       </c>
     </row>
@@ -2006,22 +2006,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>6.97</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>6.99</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>6.98</t>
-        </is>
-      </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6.96</t>
+          <t>6.93</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6.86</t>
+          <t>6.85</t>
         </is>
       </c>
     </row>
@@ -2038,17 +2038,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>6.64</t>
+          <t>6.57</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>6.57</t>
+          <t>6.60</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>6.77</t>
+          <t>6.78</t>
         </is>
       </c>
     </row>
@@ -2125,31 +2125,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-3.5444</v>
+        <v>-3.5416</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1033</v>
+        <v>0.1083</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.7341</v>
+        <v>-3.7504</v>
       </c>
       <c r="E2" t="n">
-        <v>-3.3423</v>
+        <v>-3.3454</v>
       </c>
       <c r="F2" t="n">
-        <v>0.014</v>
+        <v>0.0101</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0055</v>
+        <v>0.0041</v>
       </c>
       <c r="H2" t="n">
-        <v>55.0324</v>
+        <v>113.8286</v>
       </c>
       <c r="I2" t="n">
-        <v>169.1281</v>
+        <v>354.8834</v>
       </c>
       <c r="J2" t="n">
-        <v>1.0379</v>
+        <v>1.0385</v>
       </c>
     </row>
     <row r="3">
@@ -2159,31 +2159,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-3.6375</v>
+        <v>-3.63</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1906</v>
+        <v>0.1881</v>
       </c>
       <c r="D3" t="n">
-        <v>-4.0056</v>
+        <v>-4.0103</v>
       </c>
       <c r="E3" t="n">
-        <v>-3.2987</v>
+        <v>-3.2983</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0209</v>
+        <v>0.0138</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0124</v>
+        <v>0.0074</v>
       </c>
       <c r="H3" t="n">
-        <v>82.32940000000001</v>
+        <v>190.395</v>
       </c>
       <c r="I3" t="n">
-        <v>92.0359</v>
+        <v>314.7142</v>
       </c>
       <c r="J3" t="n">
-        <v>1.0553</v>
+        <v>1.0115</v>
       </c>
     </row>
     <row r="4">
@@ -2193,31 +2193,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.3788</v>
+        <v>1.3779</v>
       </c>
       <c r="C4" t="n">
-        <v>0.151</v>
+        <v>0.1544</v>
       </c>
       <c r="D4" t="n">
-        <v>1.1081</v>
+        <v>1.0904</v>
       </c>
       <c r="E4" t="n">
-        <v>1.6683</v>
+        <v>1.6697</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0151</v>
+        <v>0.0109</v>
       </c>
       <c r="G4" t="n">
-        <v>0.007</v>
+        <v>0.005</v>
       </c>
       <c r="H4" t="n">
-        <v>101.3883</v>
+        <v>204.743</v>
       </c>
       <c r="I4" t="n">
-        <v>266.408</v>
+        <v>463.0751</v>
       </c>
       <c r="J4" t="n">
-        <v>1.024</v>
+        <v>1.0201</v>
       </c>
     </row>
     <row r="5">
@@ -2227,31 +2227,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.217</v>
+        <v>0.2182</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2602</v>
+        <v>0.2506</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.2543</v>
+        <v>-0.2191</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6837</v>
+        <v>0.7062</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0399</v>
+        <v>0.0194</v>
       </c>
       <c r="G5" t="n">
-        <v>0.025</v>
+        <v>0.008800000000000001</v>
       </c>
       <c r="H5" t="n">
-        <v>49.3175</v>
+        <v>173.001</v>
       </c>
       <c r="I5" t="n">
-        <v>92.5549</v>
+        <v>411.5742</v>
       </c>
       <c r="J5" t="n">
-        <v>1.0754</v>
+        <v>1.0148</v>
       </c>
     </row>
     <row r="6">
@@ -2261,31 +2261,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.9116</v>
+        <v>2.9175</v>
       </c>
       <c r="C6" t="n">
-        <v>1.1705</v>
+        <v>1.1518</v>
       </c>
       <c r="D6" t="n">
-        <v>0.98</v>
+        <v>0.6529</v>
       </c>
       <c r="E6" t="n">
-        <v>5.0425</v>
+        <v>4.8772</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2164</v>
+        <v>0.133</v>
       </c>
       <c r="G6" t="n">
-        <v>0.191</v>
+        <v>0.062</v>
       </c>
       <c r="H6" t="n">
-        <v>28.2635</v>
+        <v>71.2413</v>
       </c>
       <c r="I6" t="n">
-        <v>28.4597</v>
+        <v>120.026</v>
       </c>
       <c r="J6" t="n">
-        <v>1.1032</v>
+        <v>1.0543</v>
       </c>
     </row>
   </sheetData>
@@ -2361,31 +2361,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-3.64</v>
+        <v>-3.6281</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1254</v>
+        <v>0.1247</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.8672</v>
+        <v>-3.8647</v>
       </c>
       <c r="E2" t="n">
-        <v>-3.3988</v>
+        <v>-3.3942</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0226</v>
+        <v>0.0124</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0044</v>
+        <v>0.0055</v>
       </c>
       <c r="H2" t="n">
-        <v>30.9104</v>
+        <v>102.1082</v>
       </c>
       <c r="I2" t="n">
-        <v>244.0368</v>
+        <v>281.344</v>
       </c>
       <c r="J2" t="n">
-        <v>1.0877</v>
+        <v>1.0205</v>
       </c>
     </row>
     <row r="3">
@@ -2395,31 +2395,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2056</v>
+        <v>0.2027</v>
       </c>
       <c r="C3" t="n">
-        <v>0.057</v>
+        <v>0.0594</v>
       </c>
       <c r="D3" t="n">
-        <v>0.091</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3069</v>
+        <v>0.3087</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0031</v>
+        <v>0.0024</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0013</v>
+        <v>0.0015</v>
       </c>
       <c r="H3" t="n">
-        <v>348.7436</v>
+        <v>632.8017</v>
       </c>
       <c r="I3" t="n">
-        <v>710.9018</v>
+        <v>792.3817</v>
       </c>
       <c r="J3" t="n">
-        <v>1.0133</v>
+        <v>1.0072</v>
       </c>
     </row>
     <row r="4">
@@ -2429,31 +2429,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.1051</v>
+        <v>-0.1054</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0743</v>
+        <v>0.077</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2497</v>
+        <v>-0.253</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0303</v>
+        <v>0.0378</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0023</v>
+        <v>0.0019</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0016</v>
+        <v>0.0015</v>
       </c>
       <c r="H4" t="n">
-        <v>1063.5685</v>
+        <v>1663.0821</v>
       </c>
       <c r="I4" t="n">
-        <v>1859.6704</v>
+        <v>2729.5265</v>
       </c>
       <c r="J4" t="n">
-        <v>1.0074</v>
+        <v>1.0023</v>
       </c>
     </row>
     <row r="5">
@@ -2463,31 +2463,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.08400000000000001</v>
+        <v>0.0801</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0927</v>
+        <v>0.09859999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0887</v>
+        <v>-0.1036</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2634</v>
+        <v>0.2666</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0043</v>
+        <v>0.0037</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0021</v>
+        <v>0.0023</v>
       </c>
       <c r="H5" t="n">
-        <v>461.2482</v>
+        <v>731.5786000000001</v>
       </c>
       <c r="I5" t="n">
-        <v>1018.5832</v>
+        <v>1008.0976</v>
       </c>
       <c r="J5" t="n">
-        <v>1.0052</v>
+        <v>1.0093</v>
       </c>
     </row>
     <row r="6">
@@ -2497,31 +2497,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-3.9504</v>
+        <v>-3.9483</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2648</v>
+        <v>0.2734</v>
       </c>
       <c r="D6" t="n">
-        <v>-4.4472</v>
+        <v>-4.4482</v>
       </c>
       <c r="E6" t="n">
-        <v>-3.4679</v>
+        <v>-3.4625</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0381</v>
+        <v>0.0262</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0154</v>
+        <v>0.0153</v>
       </c>
       <c r="H6" t="n">
-        <v>48.8896</v>
+        <v>115.4453</v>
       </c>
       <c r="I6" t="n">
-        <v>186.3261</v>
+        <v>278.4746</v>
       </c>
       <c r="J6" t="n">
-        <v>1.0679</v>
+        <v>1.0406</v>
       </c>
     </row>
     <row r="7">
@@ -2531,31 +2531,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0486</v>
+        <v>0.0353</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1299</v>
+        <v>0.1512</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.2</v>
+        <v>-0.2394</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2886</v>
+        <v>0.299</v>
       </c>
       <c r="F7" t="n">
-        <v>0.007900000000000001</v>
+        <v>0.0078</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0052</v>
+        <v>0.0141</v>
       </c>
       <c r="H7" t="n">
-        <v>268.9322</v>
+        <v>454.9572</v>
       </c>
       <c r="I7" t="n">
-        <v>402.8904</v>
+        <v>271.6116</v>
       </c>
       <c r="J7" t="n">
-        <v>1.0221</v>
+        <v>1.0133</v>
       </c>
     </row>
     <row r="8">
@@ -2565,31 +2565,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.09669999999999999</v>
+        <v>0.1015</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1068</v>
+        <v>0.1156</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1011</v>
+        <v>-0.1153</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2961</v>
+        <v>0.3192</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0059</v>
+        <v>0.005</v>
       </c>
       <c r="G8" t="n">
-        <v>0.003</v>
+        <v>0.0027</v>
       </c>
       <c r="H8" t="n">
-        <v>322.6393</v>
+        <v>521.888</v>
       </c>
       <c r="I8" t="n">
-        <v>629.7186</v>
+        <v>1069.8731</v>
       </c>
       <c r="J8" t="n">
-        <v>1.0217</v>
+        <v>1.006</v>
       </c>
     </row>
     <row r="9">
@@ -2599,31 +2599,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.4295</v>
+        <v>0.4145</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2289</v>
+        <v>0.2516</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0081</v>
+        <v>-0.0462</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8832</v>
+        <v>0.8924</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0141</v>
+        <v>0.0126</v>
       </c>
       <c r="G9" t="n">
-        <v>0.008</v>
+        <v>0.008800000000000001</v>
       </c>
       <c r="H9" t="n">
-        <v>265.7637</v>
+        <v>418.9069</v>
       </c>
       <c r="I9" t="n">
-        <v>546.0699</v>
+        <v>645.8927</v>
       </c>
       <c r="J9" t="n">
-        <v>1.0103</v>
+        <v>1.017</v>
       </c>
     </row>
     <row r="10">
@@ -2633,31 +2633,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.3803</v>
+        <v>1.3756</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1672</v>
+        <v>0.174</v>
       </c>
       <c r="D10" t="n">
-        <v>1.0688</v>
+        <v>1.069</v>
       </c>
       <c r="E10" t="n">
-        <v>1.6917</v>
+        <v>1.716</v>
       </c>
       <c r="F10" t="n">
-        <v>0.029</v>
+        <v>0.0164</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0068</v>
+        <v>0.0095</v>
       </c>
       <c r="H10" t="n">
-        <v>32.6989</v>
+        <v>114.4889</v>
       </c>
       <c r="I10" t="n">
-        <v>205.9711</v>
+        <v>267.258</v>
       </c>
       <c r="J10" t="n">
-        <v>1.0876</v>
+        <v>1.0275</v>
       </c>
     </row>
     <row r="11">
@@ -2667,31 +2667,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.2055</v>
+        <v>0.2291</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2367</v>
+        <v>0.2868</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.2348</v>
+        <v>-0.2643</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6422</v>
+        <v>0.7324000000000001</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0303</v>
+        <v>0.0276</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0149</v>
+        <v>0.0267</v>
       </c>
       <c r="H11" t="n">
-        <v>57.7232</v>
+        <v>139.5045</v>
       </c>
       <c r="I11" t="n">
-        <v>136.898</v>
+        <v>246.119</v>
       </c>
       <c r="J11" t="n">
-        <v>1.0641</v>
+        <v>1.0435</v>
       </c>
     </row>
     <row r="12">
@@ -2701,31 +2701,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2.3503</v>
+        <v>2.5216</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0039</v>
+        <v>1.1156</v>
       </c>
       <c r="D12" t="n">
-        <v>0.668</v>
+        <v>0.6482</v>
       </c>
       <c r="E12" t="n">
-        <v>4.3239</v>
+        <v>4.5704</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1511</v>
+        <v>0.1745</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0717</v>
+        <v>0.1302</v>
       </c>
       <c r="H12" t="n">
-        <v>40.4364</v>
+        <v>38.8707</v>
       </c>
       <c r="I12" t="n">
-        <v>97.0141</v>
+        <v>87.02249999999999</v>
       </c>
       <c r="J12" t="n">
-        <v>1.0794</v>
+        <v>1.0623</v>
       </c>
     </row>
   </sheetData>
@@ -2801,31 +2801,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-3.5331</v>
+        <v>-3.5451</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1106</v>
+        <v>0.1058</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.7339</v>
+        <v>-3.749</v>
       </c>
       <c r="E2" t="n">
-        <v>-3.3262</v>
+        <v>-3.343</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0209</v>
+        <v>0.0121</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0067</v>
+        <v>0.0045</v>
       </c>
       <c r="H2" t="n">
-        <v>28.4573</v>
+        <v>78.1135</v>
       </c>
       <c r="I2" t="n">
-        <v>115.1459</v>
+        <v>230.6644</v>
       </c>
       <c r="J2" t="n">
-        <v>1.1</v>
+        <v>1.0578</v>
       </c>
     </row>
     <row r="3">
@@ -2835,31 +2835,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-3.6239</v>
+        <v>-3.6385</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1963</v>
+        <v>0.2137</v>
       </c>
       <c r="D3" t="n">
-        <v>-3.9877</v>
+        <v>-4.0265</v>
       </c>
       <c r="E3" t="n">
-        <v>-3.2549</v>
+        <v>-3.2567</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0219</v>
+        <v>0.0217</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0143</v>
+        <v>0.0164</v>
       </c>
       <c r="H3" t="n">
-        <v>81.2829</v>
+        <v>75.104</v>
       </c>
       <c r="I3" t="n">
-        <v>140.7322</v>
+        <v>144.4383</v>
       </c>
       <c r="J3" t="n">
-        <v>1.0492</v>
+        <v>1.0481</v>
       </c>
     </row>
     <row r="4">
@@ -2869,31 +2869,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.2314</v>
+        <v>3.2324</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0149</v>
+        <v>0.0153</v>
       </c>
       <c r="D4" t="n">
-        <v>3.2022</v>
+        <v>3.2034</v>
       </c>
       <c r="E4" t="n">
-        <v>3.2582</v>
+        <v>3.2609</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0004</v>
+        <v>0.0003</v>
       </c>
       <c r="G4" t="n">
         <v>0.0002</v>
       </c>
       <c r="H4" t="n">
-        <v>1499.9869</v>
+        <v>2658.304</v>
       </c>
       <c r="I4" t="n">
-        <v>3149.9149</v>
+        <v>5374.2347</v>
       </c>
       <c r="J4" t="n">
-        <v>1.0011</v>
+        <v>1.0019</v>
       </c>
     </row>
     <row r="5">
@@ -2903,31 +2903,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.3561</v>
+        <v>1.3728</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1565</v>
+        <v>0.1665</v>
       </c>
       <c r="D5" t="n">
-        <v>1.0612</v>
+        <v>1.0749</v>
       </c>
       <c r="E5" t="n">
-        <v>1.6539</v>
+        <v>1.6888</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0152</v>
+        <v>0.0202</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0074</v>
+        <v>0.0086</v>
       </c>
       <c r="H5" t="n">
-        <v>104.6756</v>
+        <v>65.5519</v>
       </c>
       <c r="I5" t="n">
-        <v>192.2475</v>
+        <v>218.6859</v>
       </c>
       <c r="J5" t="n">
-        <v>1.0205</v>
+        <v>1.0514</v>
       </c>
     </row>
     <row r="6">
@@ -2937,31 +2937,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2242</v>
+        <v>0.2241</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2678</v>
+        <v>0.259</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.2462</v>
+        <v>-0.2506</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7141</v>
+        <v>0.6883</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0506</v>
+        <v>0.0218</v>
       </c>
       <c r="G6" t="n">
-        <v>0.04</v>
+        <v>0.0162</v>
       </c>
       <c r="H6" t="n">
-        <v>38.5095</v>
+        <v>148.2998</v>
       </c>
       <c r="I6" t="n">
-        <v>34.83</v>
+        <v>231.7239</v>
       </c>
       <c r="J6" t="n">
-        <v>1.0935</v>
+        <v>1.0186</v>
       </c>
     </row>
     <row r="7">
@@ -2977,25 +2977,25 @@
         <v>0.009900000000000001</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0054</v>
+        <v>-0.0053</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0318</v>
+        <v>0.032</v>
       </c>
       <c r="F7" t="n">
         <v>0.0001</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>6127.531</v>
+        <v>16986.6943</v>
       </c>
       <c r="I7" t="n">
-        <v>12502.7976</v>
+        <v>20605.3468</v>
       </c>
       <c r="J7" t="n">
-        <v>1.0014</v>
+        <v>1.0005</v>
       </c>
     </row>
     <row r="8">
@@ -3005,31 +3005,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.8646</v>
+        <v>2.702</v>
       </c>
       <c r="C8" t="n">
-        <v>1.2543</v>
+        <v>1.0448</v>
       </c>
       <c r="D8" t="n">
-        <v>1.0011</v>
+        <v>0.9824000000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>5.367</v>
+        <v>4.6564</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3966</v>
+        <v>0.1103</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1627</v>
+        <v>0.0658</v>
       </c>
       <c r="H8" t="n">
-        <v>11.0432</v>
+        <v>89.0046</v>
       </c>
       <c r="I8" t="n">
-        <v>66.8747</v>
+        <v>208.2597</v>
       </c>
       <c r="J8" t="n">
-        <v>1.2849</v>
+        <v>1.0322</v>
       </c>
     </row>
     <row r="9">
@@ -3039,31 +3039,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.008200000000000001</v>
+        <v>-0.0078</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0147</v>
+        <v>0.0141</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.0368</v>
+        <v>-0.0348</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0188</v>
+        <v>0.0184</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0004</v>
+        <v>0.0003</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0009</v>
+        <v>0.0002</v>
       </c>
       <c r="H9" t="n">
-        <v>1379.3299</v>
+        <v>2041.4686</v>
       </c>
       <c r="I9" t="n">
-        <v>636.0331</v>
+        <v>2769.0468</v>
       </c>
       <c r="J9" t="n">
-        <v>1.0141</v>
+        <v>1.0042</v>
       </c>
     </row>
     <row r="10">
@@ -3076,28 +3076,28 @@
         <v>0.08450000000000001</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0098</v>
+        <v>0.0095</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0667</v>
+        <v>0.06710000000000001</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1033</v>
+        <v>0.1027</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0004</v>
+        <v>0.0003</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0002</v>
+        <v>0.0001</v>
       </c>
       <c r="H10" t="n">
-        <v>510.1431</v>
+        <v>1154.3864</v>
       </c>
       <c r="I10" t="n">
-        <v>1001.5409</v>
+        <v>2482.7616</v>
       </c>
       <c r="J10" t="n">
-        <v>1.0083</v>
+        <v>1.0033</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Convergence for Tri M2
</commit_message>
<xml_diff>
--- a/outputs/excel/x_comparison_four_models.xlsx
+++ b/outputs/excel/x_comparison_four_models.xlsx
@@ -551,7 +551,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,204 +711,408 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>level_2[var_log_lambda]</t>
+          <t>level_2[beta_lambda[0]]</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.3893</v>
+        <v>-3.8665</v>
       </c>
       <c r="C5" t="n">
-        <v>0.162</v>
+        <v>0.2175</v>
       </c>
       <c r="D5" t="n">
-        <v>1.0976</v>
+        <v>-4.2798</v>
       </c>
       <c r="E5" t="n">
-        <v>1.7093</v>
+        <v>-3.4672</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0145</v>
+        <v>0.0175</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0049</v>
+        <v>0.0071</v>
       </c>
       <c r="H5" t="n">
-        <v>124.3793</v>
+        <v>153.3986</v>
       </c>
       <c r="I5" t="n">
-        <v>408.853</v>
+        <v>481.8686</v>
       </c>
       <c r="J5" t="n">
-        <v>1.042</v>
+        <v>1.0288</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>level_2[cov_log_lambda_mu]</t>
+          <t>level_2[beta_mu[0]]</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1718</v>
+        <v>0.0993</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2085</v>
+        <v>0.1037</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.2143</v>
+        <v>-0.0982</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5675</v>
+        <v>0.2948</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0153</v>
+        <v>0.0042</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0078</v>
+        <v>0.0024</v>
       </c>
       <c r="H6" t="n">
-        <v>182.3889</v>
+        <v>614.7891</v>
       </c>
       <c r="I6" t="n">
-        <v>428.4539</v>
+        <v>1287.8694</v>
       </c>
       <c r="J6" t="n">
-        <v>1.0241</v>
+        <v>1.0081</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>level_2[cov_log_lambda_eta]</t>
+          <t>level_2[beta_eta[0]]</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0151</v>
+        <v>0.3791</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0105</v>
+        <v>0.1938</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0044</v>
+        <v>0.0135</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0352</v>
+        <v>0.7495000000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0001</v>
+        <v>0.0086</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.0058</v>
       </c>
       <c r="H7" t="n">
-        <v>10735.968</v>
+        <v>509.1998</v>
       </c>
       <c r="I7" t="n">
-        <v>21456.001</v>
+        <v>750.3375</v>
       </c>
       <c r="J7" t="n">
-        <v>1.0019</v>
+        <v>1.0048</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>level_2[var_log_mu]</t>
+          <t>level_2[beta_lambda[1]]</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.1195</v>
+        <v>3.2135</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9838</v>
+        <v>0.08989999999999999</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4981</v>
+        <v>3.0456</v>
       </c>
       <c r="E8" t="n">
-        <v>3.9412</v>
+        <v>3.3856</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1608</v>
+        <v>0.0019</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0732</v>
+        <v>0.0009</v>
       </c>
       <c r="H8" t="n">
-        <v>36.4652</v>
+        <v>2317.3609</v>
       </c>
       <c r="I8" t="n">
-        <v>112.901</v>
+        <v>5136.2084</v>
       </c>
       <c r="J8" t="n">
-        <v>1.0934</v>
+        <v>1.0008</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>level_2[cov_log_mu_eta]</t>
+          <t>level_2[beta_mu[1]]</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.0072</v>
+        <v>0.0191</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0135</v>
+        <v>0.1087</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.0335</v>
+        <v>-0.1777</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0175</v>
+        <v>0.2304</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0004</v>
+        <v>0.002</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0004</v>
+        <v>0.0023</v>
       </c>
       <c r="H9" t="n">
-        <v>1020.2956</v>
+        <v>2903.5222</v>
       </c>
       <c r="I9" t="n">
-        <v>1310.9524</v>
+        <v>4130.3821</v>
       </c>
       <c r="J9" t="n">
-        <v>1.0063</v>
+        <v>1.0061</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
+          <t>level_2[beta_eta[1]]</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0361</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0315</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0.0242</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0936</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2831.7283</v>
+      </c>
+      <c r="I10" t="n">
+        <v>6337.3762</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.0014</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>level_2[var_log_lambda]</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1.3893</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.162</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.0976</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.7093</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0145</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0049</v>
+      </c>
+      <c r="H11" t="n">
+        <v>124.3793</v>
+      </c>
+      <c r="I11" t="n">
+        <v>408.853</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.042</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>level_2[cov_log_lambda_mu]</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.1718</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.2085</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.2143</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.5675</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0153</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0078</v>
+      </c>
+      <c r="H12" t="n">
+        <v>182.3889</v>
+      </c>
+      <c r="I12" t="n">
+        <v>428.4539</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1.0241</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>level_2[cov_log_lambda_eta]</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.0151</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0105</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.0044</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0352</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>10735.968</v>
+      </c>
+      <c r="I13" t="n">
+        <v>21456.001</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.0019</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>level_2[var_log_mu]</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2.1195</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.9838</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.4981</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.9412</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.1608</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0732</v>
+      </c>
+      <c r="H14" t="n">
+        <v>36.4652</v>
+      </c>
+      <c r="I14" t="n">
+        <v>112.901</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1.0934</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>level_2[cov_log_mu_eta]</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-0.0072</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0135</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.0335</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0175</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1020.2956</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1310.9524</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1.0063</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
           <t>level_2[var_log_eta]</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B16" t="n">
         <v>0.09470000000000001</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C16" t="n">
         <v>0.009900000000000001</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D16" t="n">
         <v>0.0766</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E16" t="n">
         <v>0.1135</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F16" t="n">
         <v>0.0003</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G16" t="n">
         <v>0.0001</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H16" t="n">
         <v>1292.2827</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I16" t="n">
         <v>2693.9331</v>
       </c>
-      <c r="J10" t="n">
+      <c r="J16" t="n">
         <v>1.0013</v>
       </c>
     </row>

</xml_diff>